<commit_message>
git commit -m "added invalid request demo method"
</commit_message>
<xml_diff>
--- a/test_data/RequestDemoData.xlsx
+++ b/test_data/RequestDemoData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arrowelectronics-my.sharepoint.com/personal/afzalkhan_inayathkhan_einfochips_com/Documents/Desktop/Python Training/Practice/Project1/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{81C27D9F-09C1-4815-87C7-11F24214C605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ED8F22A-AF4F-404E-97E6-B6FF2FDADE74}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{81C27D9F-09C1-4815-87C7-11F24214C605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CFD47EF-BDAF-4D69-9C68-13C31C49D893}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B7EF6E9-F4D9-4762-AD3B-5B9344740973}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5B7EF6E9-F4D9-4762-AD3B-5B9344740973}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid_Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>FirstName</t>
   </si>
@@ -111,6 +112,30 @@
   </si>
   <si>
     <t>dde</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>InvalidField</t>
+  </si>
+  <si>
+    <t>Work Email</t>
+  </si>
+  <si>
+    <t>ErrorMsg</t>
+  </si>
+  <si>
+    <t>Please input a valid email address.</t>
+  </si>
+  <si>
+    <t>Total Employees</t>
+  </si>
+  <si>
+    <t>Please input a valid number.</t>
   </si>
 </sst>
 </file>
@@ -174,10 +199,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0987991F-D315-4426-B56F-67F9B346BB5F}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,4 +629,145 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E2F4F8-259D-4D11-9A5B-A22F93AD8286}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>9876543210</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>9876543210</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="abcd@gmail.com" xr:uid="{F0D31DB1-B2B9-4015-97AA-27FC74930075}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{C31C4E70-640A-4ECC-9C02-07C4ED674C93}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
git commit -m "added account creation validation"
</commit_message>
<xml_diff>
--- a/test_data/RequestDemoData.xlsx
+++ b/test_data/RequestDemoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arrowelectronics-my.sharepoint.com/personal/afzalkhan_inayathkhan_einfochips_com/Documents/Desktop/Python Training/Practice/Project1/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{81C27D9F-09C1-4815-87C7-11F24214C605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CFD47EF-BDAF-4D69-9C68-13C31C49D893}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{81C27D9F-09C1-4815-87C7-11F24214C605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F37C37BF-4785-4550-91A5-82FC589FD710}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5B7EF6E9-F4D9-4762-AD3B-5B9344740973}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>